<commit_message>
lydia edited asset list and GDD
</commit_message>
<xml_diff>
--- a/Asset list.xlsx
+++ b/Asset list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -45,6 +45,63 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">background </t>
+  </si>
+  <si>
+    <t>game pieces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">paddles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">walls </t>
+  </si>
+  <si>
+    <t xml:space="preserve">button </t>
+  </si>
+  <si>
+    <t>ball sound</t>
+  </si>
+  <si>
+    <t>paddle sound</t>
+  </si>
+  <si>
+    <t>button sound</t>
+  </si>
+  <si>
+    <t>background music</t>
+  </si>
+  <si>
+    <t>start menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dying sound </t>
+  </si>
+  <si>
+    <t>winning sound</t>
+  </si>
+  <si>
+    <t>losing sound</t>
+  </si>
+  <si>
+    <t>Technical Assests</t>
+  </si>
+  <si>
+    <t>particle effects</t>
+  </si>
+  <si>
+    <t>score board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">title </t>
   </si>
 </sst>
 </file>
@@ -362,47 +419,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="1" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alex added and cleaned up Asset list.xlsx
</commit_message>
<xml_diff>
--- a/Asset list.xlsx
+++ b/Asset list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lydia.rogers\Desktop\Team 7 Pong\Pong\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexander.parsons\Desktop\Pong\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -45,6 +45,63 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Paddle Sprite</t>
+  </si>
+  <si>
+    <t>Backgrounds</t>
+  </si>
+  <si>
+    <t>Wall Sprite</t>
+  </si>
+  <si>
+    <t>Lamp Sprites</t>
+  </si>
+  <si>
+    <t>Button Sprites</t>
+  </si>
+  <si>
+    <t>Ball Sprite</t>
+  </si>
+  <si>
+    <t>Octavio</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Looping Track</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Wall Hit</t>
+  </si>
+  <si>
+    <t>Paddle Hit</t>
+  </si>
+  <si>
+    <t>End Game</t>
+  </si>
+  <si>
+    <t>Lamp Sounds</t>
+  </si>
+  <si>
+    <t>Button Click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goal </t>
   </si>
 </sst>
 </file>
@@ -60,15 +117,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -76,12 +145,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,33 +471,224 @@
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added to Asset list.xlsx
</commit_message>
<xml_diff>
--- a/Asset list.xlsx
+++ b/Asset list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -460,7 +460,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,6 +690,9 @@
       <c r="D16" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="E16" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>